<commit_message>
maj amazon + fnac
</commit_message>
<xml_diff>
--- a/lien.xlsx
+++ b/lien.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansn\Desktop\Datanomics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B93B58E-4CE0-4FD7-A3AF-683CD58A300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38E84BC-347E-4782-A6D6-45C17F25A03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="FNAC" sheetId="2" r:id="rId2"/>
+    <sheet name="DARTY" sheetId="3" r:id="rId3"/>
+    <sheet name="AMAZON" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="281">
   <si>
     <t>Principe: focus sur les 3 dernières générations de smartphones "haut-de gamme", à voir si on intègre les pliables, car ça fait déjà environ 40 smartphones sans eux</t>
   </si>
@@ -732,13 +734,145 @@
   </si>
   <si>
     <t>Link_ID</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7203764</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7719779</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7719736</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7719418</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7719868</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7719850</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7203322</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7195311</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7632347</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7632240</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7631693</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7630964</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7630875</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7631642</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7631200</t>
+  </si>
+  <si>
+    <t>https://www.darty.com/nav/extra/offres?codic=7631332</t>
+  </si>
+  <si>
+    <t>B0DGHRL7DB</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/gp/product/ajax/ref=dp_aod_ALL_mbc?asin=B07Z6RD4M9&amp;m=&amp;qid=&amp;smid=&amp;sourcecustomerorglistid=&amp;sourcecustomerorglistitemid=&amp;sr=&amp;pc=dp&amp;experienceId=aodAjaxMain</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGHSG5CD</t>
+  </si>
+  <si>
+    <t>B0DGHSG5CD</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGHY5KG8</t>
+  </si>
+  <si>
+    <t>B0DGHY5KG8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGJ4RRSD</t>
+  </si>
+  <si>
+    <t>B0DGJ4RRSD</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGHMSMST</t>
+  </si>
+  <si>
+    <t>B0DGHMSMST</t>
+  </si>
+  <si>
+    <t>B0DGHRPFTH</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGHRPFTH</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0DGHZDQ82</t>
+  </si>
+  <si>
+    <t>B0DGHZDQ82</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHX6SD96</t>
+  </si>
+  <si>
+    <t>B0CHX6SD96</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHX13YPM</t>
+  </si>
+  <si>
+    <t>B0CHX13YPM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHXFCYCR</t>
+  </si>
+  <si>
+    <t>B0CHXFCYCR</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHXFFT8Z</t>
+  </si>
+  <si>
+    <t>B0CHXFFT8Z</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHX9XFRN</t>
+  </si>
+  <si>
+    <t>B0CHX9XFRN</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHX3ZTJQ</t>
+  </si>
+  <si>
+    <t>B0CHX3ZTJQ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/dp/B0CHWZ6YYV</t>
+  </si>
+  <si>
+    <t>B0CHWZ6YYV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -823,6 +957,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -874,15 +1015,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -898,16 +1040,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -921,8 +1053,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
     <cellStyle name="Lien hypertexte 2" xfId="2" xr:uid="{B96221E2-FC06-4D3D-8879-C3FEBF5AF7DE}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{E7AD36FE-1D69-4237-8488-42B633417DB3}"/>
@@ -1143,101 +1288,100 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="7" width="15.36328125" customWidth="1"/>
-    <col min="8" max="9" width="16.36328125" customWidth="1"/>
-    <col min="10" max="11" width="14.90625" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
-    <col min="13" max="14" width="14.90625" customWidth="1"/>
-    <col min="15" max="16" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="16" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="15" t="s">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="14"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="16" t="s">
+      <c r="N7" s="23"/>
+      <c r="O7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="14"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22"/>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1280,8 +1424,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1326,8 +1470,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
@@ -1374,8 +1518,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
@@ -1418,8 +1562,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>52</v>
       </c>
@@ -1462,8 +1606,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>60</v>
       </c>
@@ -1508,8 +1652,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>69</v>
       </c>
@@ -1554,8 +1698,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
       <c r="B15" s="3" t="s">
         <v>77</v>
       </c>
@@ -1598,8 +1742,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23"/>
       <c r="B16" s="9" t="s">
         <v>83</v>
       </c>
@@ -1643,8 +1787,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
       <c r="B17" s="9" t="s">
         <v>92</v>
       </c>
@@ -1688,8 +1832,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
       <c r="B18" s="9" t="s">
         <v>101</v>
       </c>
@@ -1734,8 +1878,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="23"/>
       <c r="B19" s="9" t="s">
         <v>111</v>
       </c>
@@ -1779,8 +1923,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="23"/>
       <c r="B20" s="9" t="s">
         <v>119</v>
       </c>
@@ -1821,8 +1965,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="23"/>
       <c r="B21" s="9" t="s">
         <v>127</v>
       </c>
@@ -1866,8 +2010,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="23"/>
       <c r="B22" s="9" t="s">
         <v>136</v>
       </c>
@@ -1911,8 +2055,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="23"/>
       <c r="B23" s="9" t="s">
         <v>145</v>
       </c>
@@ -1954,8 +2098,8 @@
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="23"/>
       <c r="B24" s="4" t="s">
         <v>154</v>
       </c>
@@ -1974,8 +2118,8 @@
       <c r="O24" s="5"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+    <row r="25" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="23"/>
       <c r="B25" s="4" t="s">
         <v>155</v>
       </c>
@@ -1994,8 +2138,8 @@
       <c r="O25" s="5"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+    <row r="26" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="23"/>
       <c r="B26" s="4" t="s">
         <v>156</v>
       </c>
@@ -2014,8 +2158,8 @@
       <c r="O26" s="5"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+    <row r="27" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="23"/>
       <c r="B27" s="4" t="s">
         <v>157</v>
       </c>
@@ -2034,8 +2178,8 @@
       <c r="O27" s="5"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+    <row r="28" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>158</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2051,8 +2195,8 @@
       <c r="M28" s="10"/>
       <c r="O28" s="10"/>
     </row>
-    <row r="29" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
         <v>161</v>
       </c>
@@ -2063,8 +2207,8 @@
       <c r="M29" s="10"/>
       <c r="O29" s="10"/>
     </row>
-    <row r="30" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
         <v>162</v>
       </c>
@@ -2075,8 +2219,8 @@
       <c r="M30" s="10"/>
       <c r="O30" s="10"/>
     </row>
-    <row r="31" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+    <row r="31" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="23"/>
       <c r="B31" s="1" t="s">
         <v>163</v>
       </c>
@@ -2087,8 +2231,8 @@
       <c r="M31" s="10"/>
       <c r="O31" s="10"/>
     </row>
-    <row r="32" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+    <row r="32" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="23"/>
       <c r="B32" s="4" t="s">
         <v>164</v>
       </c>
@@ -2107,8 +2251,8 @@
       <c r="O32" s="5"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+    <row r="33" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>165</v>
       </c>
@@ -2127,8 +2271,8 @@
       <c r="O33" s="5"/>
       <c r="P33" s="4"/>
     </row>
-    <row r="34" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+    <row r="34" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="23"/>
       <c r="B34" s="4" t="s">
         <v>166</v>
       </c>
@@ -2147,8 +2291,8 @@
       <c r="O34" s="5"/>
       <c r="P34" s="4"/>
     </row>
-    <row r="35" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+    <row r="35" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="23"/>
       <c r="B35" s="4" t="s">
         <v>167</v>
       </c>
@@ -2167,8 +2311,8 @@
       <c r="O35" s="5"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+    <row r="36" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="23"/>
       <c r="B36" s="1" t="s">
         <v>168</v>
       </c>
@@ -2179,8 +2323,8 @@
       <c r="M36" s="10"/>
       <c r="O36" s="10"/>
     </row>
-    <row r="37" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+    <row r="37" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="23"/>
       <c r="B37" s="1" t="s">
         <v>169</v>
       </c>
@@ -2191,8 +2335,8 @@
       <c r="M37" s="10"/>
       <c r="O37" s="10"/>
     </row>
-    <row r="38" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+    <row r="38" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="23"/>
       <c r="B38" s="1" t="s">
         <v>170</v>
       </c>
@@ -2203,8 +2347,8 @@
       <c r="M38" s="10"/>
       <c r="O38" s="10"/>
     </row>
-    <row r="39" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+    <row r="39" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="23"/>
       <c r="B39" s="1" t="s">
         <v>171</v>
       </c>
@@ -2215,8 +2359,8 @@
       <c r="M39" s="10"/>
       <c r="O39" s="10"/>
     </row>
-    <row r="40" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    <row r="40" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
         <v>172</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -2237,8 +2381,8 @@
       <c r="O40" s="5"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+    <row r="41" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="23"/>
       <c r="B41" s="4" t="s">
         <v>174</v>
       </c>
@@ -2257,8 +2401,8 @@
       <c r="O41" s="5"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+    <row r="42" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="23"/>
       <c r="B42" s="4" t="s">
         <v>175</v>
       </c>
@@ -2277,8 +2421,8 @@
       <c r="O42" s="5"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+    <row r="43" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="23"/>
       <c r="B43" s="1" t="s">
         <v>176</v>
       </c>
@@ -2289,8 +2433,8 @@
       <c r="M43" s="10"/>
       <c r="O43" s="10"/>
     </row>
-    <row r="44" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+    <row r="44" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="23"/>
       <c r="B44" s="1" t="s">
         <v>177</v>
       </c>
@@ -2301,8 +2445,8 @@
       <c r="M44" s="10"/>
       <c r="O44" s="10"/>
     </row>
-    <row r="45" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+    <row r="45" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="23"/>
       <c r="B45" s="1" t="s">
         <v>178</v>
       </c>
@@ -2313,8 +2457,8 @@
       <c r="M45" s="10"/>
       <c r="O45" s="10"/>
     </row>
-    <row r="46" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+    <row r="46" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="23"/>
       <c r="B46" s="4" t="s">
         <v>179</v>
       </c>
@@ -2333,8 +2477,8 @@
       <c r="O46" s="5"/>
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+    <row r="47" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="23"/>
       <c r="B47" s="4" t="s">
         <v>180</v>
       </c>
@@ -2353,8 +2497,8 @@
       <c r="O47" s="5"/>
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+    <row r="48" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="23"/>
       <c r="B48" s="4" t="s">
         <v>181</v>
       </c>
@@ -2373,8 +2517,8 @@
       <c r="O48" s="5"/>
       <c r="P48" s="4"/>
     </row>
-    <row r="49" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="22" t="s">
         <v>182</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -2390,8 +2534,8 @@
       <c r="M49" s="10"/>
       <c r="O49" s="10"/>
     </row>
-    <row r="50" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+    <row r="50" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="23"/>
       <c r="B50" s="1" t="s">
         <v>185</v>
       </c>
@@ -2405,8 +2549,8 @@
       <c r="M50" s="10"/>
       <c r="O50" s="10"/>
     </row>
-    <row r="51" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+    <row r="51" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="23"/>
       <c r="B51" s="4" t="s">
         <v>186</v>
       </c>
@@ -2425,8 +2569,8 @@
       <c r="O51" s="5"/>
       <c r="P51" s="4"/>
     </row>
-    <row r="52" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
+    <row r="52" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="23"/>
       <c r="B52" s="4" t="s">
         <v>187</v>
       </c>
@@ -2445,8 +2589,8 @@
       <c r="O52" s="5"/>
       <c r="P52" s="4"/>
     </row>
-    <row r="53" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
+    <row r="53" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="23"/>
       <c r="B53" s="4" t="s">
         <v>188</v>
       </c>
@@ -2465,8 +2609,8 @@
       <c r="O53" s="5"/>
       <c r="P53" s="4"/>
     </row>
-    <row r="54" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+    <row r="54" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="23"/>
       <c r="B54" s="1" t="s">
         <v>189</v>
       </c>
@@ -2477,8 +2621,8 @@
       <c r="M54" s="10"/>
       <c r="O54" s="10"/>
     </row>
-    <row r="55" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+    <row r="55" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="23"/>
       <c r="B55" s="1" t="s">
         <v>190</v>
       </c>
@@ -2489,8 +2633,8 @@
       <c r="M55" s="10"/>
       <c r="O55" s="10"/>
     </row>
-    <row r="56" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+    <row r="56" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="23"/>
       <c r="B56" s="1" t="s">
         <v>191</v>
       </c>
@@ -2501,58 +2645,58 @@
       <c r="M56" s="10"/>
       <c r="O56" s="10"/>
     </row>
-    <row r="57" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J57" s="10"/>
       <c r="M57" s="10"/>
       <c r="O57" s="10"/>
     </row>
-    <row r="60" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="22" t="s">
         <v>158</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+    <row r="63" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="23"/>
       <c r="B63" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+    <row r="64" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="23"/>
       <c r="B64" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+    <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="22" t="s">
         <v>172</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+    <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="23"/>
       <c r="B66" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
+    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="23"/>
       <c r="B67" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+    <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="22" t="s">
         <v>182</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -2562,8 +2706,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+    <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="23"/>
       <c r="B69" s="1" t="s">
         <v>201</v>
       </c>
@@ -2571,8 +2715,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+    <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="23"/>
       <c r="B70" s="1" t="s">
         <v>202</v>
       </c>
@@ -2708,252 +2852,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AACF13-4D53-41D8-93BE-04E10BC12909}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.90625" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="21" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:4" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="14" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>92</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="14" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>111</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>127</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="14" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>136</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="14" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>145</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="14" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2977,4 +3121,519 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4002AA-784C-4FFA-9E33-C7D025FF3B4F}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2">
+        <v>7203764</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3">
+        <v>7719779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="21">
+        <v>7719736</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="21">
+        <v>7719418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="21">
+        <v>7719868</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="21">
+        <v>7719850</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" s="21">
+        <v>7203322</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9">
+        <v>7195311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" s="21">
+        <v>7632347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="21">
+        <v>7632240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D12" s="21">
+        <v>7631693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="21">
+        <v>7630964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="9">
+        <v>7630875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D15" s="21">
+        <v>7631642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="21">
+        <v>7631200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="21">
+        <v>7631332</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{955AF268-F3BA-4145-82F4-2D34C8059E5F}"/>
+    <hyperlink ref="D4" r:id="rId2" display="android-app://com.darty.android.tablette/darty/produit?codic=7719736" xr:uid="{377335B8-2190-43FA-A743-21E835A5FFC3}"/>
+    <hyperlink ref="D5" r:id="rId3" display="android-app://com.darty.android.tablette/darty/produit?codic=7719418" xr:uid="{A23222F0-10C4-456F-910D-13F0D1790B1F}"/>
+    <hyperlink ref="D6" r:id="rId4" display="android-app://com.darty.android.tablette/darty/produit?codic=7719868" xr:uid="{5812998F-B533-4B05-8BE7-5904ACA2247A}"/>
+    <hyperlink ref="D7" r:id="rId5" display="android-app://com.darty.android.tablette/darty/produit?codic=7719850" xr:uid="{17D04C71-AE65-4F66-B494-7C71EFF030C9}"/>
+    <hyperlink ref="D8" r:id="rId6" display="android-app://com.darty.android.tablette/darty/produit?codic=7203322" xr:uid="{3DC11585-E1F4-47B7-A51B-41A767128ADE}"/>
+    <hyperlink ref="D10" r:id="rId7" display="android-app://com.darty.android.tablette/darty/produit?codic=7632347" xr:uid="{5E71C0EF-D28A-4D6A-83ED-907FBAE82E9F}"/>
+    <hyperlink ref="D11" r:id="rId8" display="android-app://com.darty.android.tablette/darty/produit?codic=7632240" xr:uid="{BBABB7E7-97BC-41D5-823F-20D1328688B6}"/>
+    <hyperlink ref="D12" r:id="rId9" display="android-app://com.darty.android.tablette/darty/produit?codic=7631693" xr:uid="{824646E7-AA49-4F91-9D68-555431059E4E}"/>
+    <hyperlink ref="D13" r:id="rId10" display="android-app://com.darty.android.tablette/darty/produit?codic=7630964" xr:uid="{C351F2F1-5FD6-4BCD-BA4D-EF3FBF37FD2A}"/>
+    <hyperlink ref="D15" r:id="rId11" display="android-app://com.darty.android.tablette/darty/produit?codic=7631642" xr:uid="{6E715E44-D68A-4453-B5F1-C749F4BECC55}"/>
+    <hyperlink ref="D16" r:id="rId12" display="android-app://com.darty.android.tablette/darty/produit?codic=7631200" xr:uid="{7C0E7B26-CCBC-419D-BBA9-94D23BD8ADA6}"/>
+    <hyperlink ref="D17" r:id="rId13" display="android-app://com.darty.android.tablette/darty/produit?codic=7631332" xr:uid="{7A2A1AF8-DDE9-40DB-99EB-82594FAC9ABF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B14B20-B821-4905-AA0E-0D96EE6B8932}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>257</v>
+      </c>
+      <c r="D4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="10"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{68AE2545-D160-4EA2-AF18-CCA971FC4347}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>